<commit_message>
minor changes relational schema
</commit_message>
<xml_diff>
--- a/public/imgDokumentationDWP/Relationales Schema.xlsx
+++ b/public/imgDokumentationDWP/Relationales Schema.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\Projekt\ws2425_dwp_wachs_herpe_burger\public\imgDokumentationDWP\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{84D072C8-9698-4918-9CE2-195B9A1CC838}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D846B7C-9EB5-4826-9A98-20A850893F0E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="25695" yWindow="0" windowWidth="26010" windowHeight="20985" xr2:uid="{60A825A8-C428-49F5-B227-5490875001C8}"/>
   </bookViews>
@@ -41,9 +41,6 @@
     <t>Relationales Schema:</t>
   </si>
   <si>
-    <t xml:space="preserve">                   Ort, Beschreibung, Kontaktaufnahme, Bildadresse, Gelöscht, ZuletztGeändert)</t>
-  </si>
-  <si>
     <r>
       <rPr>
         <sz val="11"/>
@@ -807,6 +804,9 @@
       </rPr>
       <t>, Art)</t>
     </r>
+  </si>
+  <si>
+    <t xml:space="preserve">             Ort, Beschreibung, Kontaktaufnahme, Bildadresse, Gelöscht, ZuletztGeändert)</t>
   </si>
 </sst>
 </file>
@@ -878,20 +878,20 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1230,7 +1230,7 @@
   <dimension ref="A2:S62"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" topLeftCell="A8" zoomScale="98" zoomScaleNormal="98" workbookViewId="0">
-      <selection activeCell="L25" sqref="L25"/>
+      <selection activeCell="U53" sqref="U53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1249,35 +1249,35 @@
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="2"/>
-      <c r="B4" s="5"/>
-      <c r="C4" s="5"/>
+      <c r="B4" s="9"/>
+      <c r="C4" s="9"/>
       <c r="D4" s="2"/>
       <c r="H4" s="2"/>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="3"/>
-      <c r="B5" s="4"/>
-      <c r="C5" s="4"/>
+      <c r="B5" s="7"/>
+      <c r="C5" s="7"/>
       <c r="D5" s="3"/>
       <c r="H5" s="3"/>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="3"/>
-      <c r="B6" s="4"/>
-      <c r="C6" s="4"/>
+      <c r="B6" s="7"/>
+      <c r="C6" s="7"/>
       <c r="D6" s="3"/>
       <c r="H6" s="2"/>
     </row>
     <row r="7" spans="1:9" ht="18" x14ac:dyDescent="0.25">
       <c r="A7" s="2"/>
-      <c r="B7" s="4"/>
-      <c r="C7" s="4"/>
+      <c r="B7" s="7"/>
+      <c r="C7" s="7"/>
       <c r="D7" s="3"/>
-      <c r="F7" s="7" t="s">
+      <c r="F7" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="G7" s="7"/>
-      <c r="H7" s="7"/>
+      <c r="G7" s="8"/>
+      <c r="H7" s="8"/>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="D8" s="2"/>
@@ -1286,39 +1286,39 @@
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" s="1"/>
-      <c r="B9" s="5"/>
-      <c r="C9" s="5"/>
+      <c r="B9" s="9"/>
+      <c r="C9" s="9"/>
       <c r="D9" s="2"/>
-      <c r="E9" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="F9" s="4"/>
-      <c r="G9" s="4"/>
-      <c r="H9" s="4"/>
+      <c r="E9" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="F9" s="7"/>
+      <c r="G9" s="7"/>
+      <c r="H9" s="7"/>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" s="2"/>
       <c r="D10" s="2"/>
-      <c r="F10" s="6"/>
+      <c r="F10" s="5"/>
       <c r="H10" s="3"/>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="D11" s="2"/>
-      <c r="F11" s="8" t="s">
-        <v>2</v>
-      </c>
-      <c r="G11" s="8"/>
-      <c r="H11" s="8"/>
+      <c r="F11" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="G11" s="6"/>
+      <c r="H11" s="6"/>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" s="1"/>
       <c r="D12" s="2"/>
-      <c r="F12" s="8" t="s">
-        <v>3</v>
-      </c>
-      <c r="G12" s="8"/>
-      <c r="H12" s="8"/>
-      <c r="I12" s="8"/>
+      <c r="F12" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="G12" s="6"/>
+      <c r="H12" s="6"/>
+      <c r="I12" s="6"/>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" s="2"/>
@@ -1328,12 +1328,12 @@
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" s="3"/>
       <c r="D14" s="1"/>
-      <c r="E14" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="F14" s="4"/>
-      <c r="G14" s="4"/>
-      <c r="H14" s="4"/>
+      <c r="E14" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="F14" s="7"/>
+      <c r="G14" s="7"/>
+      <c r="H14" s="7"/>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" s="2"/>
@@ -1344,11 +1344,11 @@
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" s="2"/>
       <c r="D16" s="2"/>
-      <c r="F16" s="8" t="s">
-        <v>4</v>
-      </c>
-      <c r="G16" s="8"/>
-      <c r="H16" s="8"/>
+      <c r="F16" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="G16" s="6"/>
+      <c r="H16" s="6"/>
     </row>
     <row r="17" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A17" s="2"/>
@@ -1358,40 +1358,40 @@
     </row>
     <row r="18" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A18" s="2"/>
-      <c r="E18" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="F18" s="4"/>
-      <c r="G18" s="4"/>
-      <c r="H18" s="4"/>
-      <c r="I18" s="4"/>
-      <c r="J18" s="4"/>
-      <c r="K18" s="4"/>
-      <c r="L18" s="4"/>
+      <c r="E18" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="F18" s="7"/>
+      <c r="G18" s="7"/>
+      <c r="H18" s="7"/>
+      <c r="I18" s="7"/>
+      <c r="J18" s="7"/>
+      <c r="K18" s="7"/>
+      <c r="L18" s="7"/>
     </row>
     <row r="19" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A19" s="2"/>
       <c r="D19" s="3"/>
-      <c r="F19" s="6"/>
+      <c r="F19" s="5"/>
     </row>
     <row r="20" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A20" s="3"/>
       <c r="D20" s="2"/>
-      <c r="F20" s="8" t="s">
-        <v>5</v>
-      </c>
-      <c r="G20" s="8"/>
-      <c r="H20" s="8"/>
+      <c r="F20" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="G20" s="6"/>
+      <c r="H20" s="6"/>
     </row>
     <row r="21" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A21" s="2"/>
       <c r="D21" s="1"/>
-      <c r="F21" s="8" t="s">
-        <v>3</v>
-      </c>
-      <c r="G21" s="8"/>
-      <c r="H21" s="8"/>
-      <c r="I21" s="8"/>
+      <c r="F21" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="G21" s="6"/>
+      <c r="H21" s="6"/>
+      <c r="I21" s="6"/>
     </row>
     <row r="22" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A22" s="2"/>
@@ -1401,14 +1401,14 @@
     <row r="23" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A23" s="2"/>
       <c r="D23" s="3"/>
-      <c r="E23" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="F23" s="4"/>
-      <c r="G23" s="4"/>
-      <c r="H23" s="4"/>
-      <c r="I23" s="4"/>
-      <c r="J23" s="4"/>
+      <c r="E23" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="F23" s="7"/>
+      <c r="G23" s="7"/>
+      <c r="H23" s="7"/>
+      <c r="I23" s="7"/>
+      <c r="J23" s="7"/>
     </row>
     <row r="24" spans="1:19" x14ac:dyDescent="0.25">
       <c r="D24" s="3"/>
@@ -1416,268 +1416,291 @@
     </row>
     <row r="25" spans="1:19" x14ac:dyDescent="0.25">
       <c r="D25" s="2"/>
-      <c r="F25" s="8" t="s">
-        <v>6</v>
-      </c>
-      <c r="G25" s="8"/>
-      <c r="H25" s="8"/>
+      <c r="F25" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="G25" s="6"/>
+      <c r="H25" s="6"/>
     </row>
     <row r="26" spans="1:19" x14ac:dyDescent="0.25">
       <c r="D26" s="2"/>
-      <c r="F26" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="G26" s="8"/>
-      <c r="H26" s="8"/>
-      <c r="I26" s="8"/>
+      <c r="F26" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="G26" s="6"/>
+      <c r="H26" s="6"/>
+      <c r="I26" s="6"/>
     </row>
     <row r="27" spans="1:19" x14ac:dyDescent="0.25">
       <c r="F27" s="2"/>
     </row>
     <row r="28" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="E28" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="F28" s="4"/>
-      <c r="G28" s="4"/>
-      <c r="H28" s="4"/>
-      <c r="I28" s="4"/>
-      <c r="J28" s="4"/>
-      <c r="K28" s="4"/>
-      <c r="L28" s="4"/>
-      <c r="M28" s="4"/>
-      <c r="N28" s="4"/>
-      <c r="O28" s="4"/>
-      <c r="P28" s="4"/>
-      <c r="Q28" s="4"/>
-      <c r="R28" s="4"/>
-      <c r="S28" s="4"/>
+      <c r="E28" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="F28" s="7"/>
+      <c r="G28" s="7"/>
+      <c r="H28" s="7"/>
+      <c r="I28" s="7"/>
+      <c r="J28" s="7"/>
+      <c r="K28" s="7"/>
+      <c r="L28" s="7"/>
+      <c r="M28" s="7"/>
+      <c r="N28" s="7"/>
+      <c r="O28" s="7"/>
+      <c r="P28" s="7"/>
+      <c r="Q28" s="7"/>
+      <c r="R28" s="7"/>
+      <c r="S28" s="7"/>
     </row>
     <row r="29" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="E29" s="9"/>
-      <c r="F29" s="9"/>
-      <c r="G29" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="H29" s="4"/>
-      <c r="I29" s="4"/>
-      <c r="J29" s="4"/>
-      <c r="K29" s="4"/>
-      <c r="L29" s="4"/>
-      <c r="M29" s="4"/>
-      <c r="N29" s="4"/>
-      <c r="O29" s="9"/>
-      <c r="P29" s="9"/>
-      <c r="Q29" s="9"/>
-      <c r="R29" s="9"/>
-      <c r="S29" s="9"/>
+      <c r="E29" s="4"/>
+      <c r="F29" s="4"/>
+      <c r="G29" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="H29" s="7"/>
+      <c r="I29" s="7"/>
+      <c r="J29" s="7"/>
+      <c r="K29" s="7"/>
+      <c r="L29" s="7"/>
+      <c r="M29" s="7"/>
+      <c r="N29" s="7"/>
+      <c r="O29" s="4"/>
+      <c r="P29" s="4"/>
+      <c r="Q29" s="4"/>
+      <c r="R29" s="4"/>
+      <c r="S29" s="4"/>
     </row>
     <row r="30" spans="1:19" x14ac:dyDescent="0.25">
       <c r="F30" s="2"/>
     </row>
     <row r="31" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="F31" s="8" t="s">
+      <c r="F31" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="G31" s="6"/>
+      <c r="H31" s="6"/>
+      <c r="I31" s="6"/>
+    </row>
+    <row r="32" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="F32" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="G32" s="6"/>
+      <c r="H32" s="6"/>
+      <c r="I32" s="6"/>
+    </row>
+    <row r="33" spans="5:12" x14ac:dyDescent="0.25">
+      <c r="F33" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="G31" s="8"/>
-      <c r="H31" s="8"/>
-      <c r="I31" s="8"/>
-    </row>
-    <row r="32" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="F32" s="8" t="s">
-        <v>3</v>
-      </c>
-      <c r="G32" s="8"/>
-      <c r="H32" s="8"/>
-      <c r="I32" s="8"/>
-    </row>
-    <row r="33" spans="5:12" x14ac:dyDescent="0.25">
-      <c r="F33" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="G33" s="8"/>
-      <c r="H33" s="8"/>
-      <c r="I33" s="8"/>
-      <c r="J33" s="8"/>
+      <c r="G33" s="6"/>
+      <c r="H33" s="6"/>
+      <c r="I33" s="6"/>
+      <c r="J33" s="6"/>
     </row>
     <row r="34" spans="5:12" x14ac:dyDescent="0.25">
       <c r="F34" s="2"/>
     </row>
     <row r="35" spans="5:12" x14ac:dyDescent="0.25">
-      <c r="E35" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="F35" s="4"/>
-      <c r="G35" s="4"/>
-      <c r="H35" s="4"/>
-      <c r="I35" s="4"/>
-      <c r="J35" s="4"/>
+      <c r="E35" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="F35" s="7"/>
+      <c r="G35" s="7"/>
+      <c r="H35" s="7"/>
+      <c r="I35" s="7"/>
+      <c r="J35" s="7"/>
     </row>
     <row r="36" spans="5:12" x14ac:dyDescent="0.25">
       <c r="F36" s="2"/>
     </row>
     <row r="37" spans="5:12" x14ac:dyDescent="0.25">
-      <c r="F37" s="8" t="s">
+      <c r="F37" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="G37" s="6"/>
+      <c r="H37" s="6"/>
+    </row>
+    <row r="38" spans="5:12" x14ac:dyDescent="0.25">
+      <c r="F38" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="G37" s="8"/>
-      <c r="H37" s="8"/>
-    </row>
-    <row r="38" spans="5:12" x14ac:dyDescent="0.25">
-      <c r="F38" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="G38" s="4"/>
-      <c r="H38" s="4"/>
-      <c r="I38" s="4"/>
-      <c r="J38" s="4"/>
+      <c r="G38" s="7"/>
+      <c r="H38" s="7"/>
+      <c r="I38" s="7"/>
+      <c r="J38" s="7"/>
     </row>
     <row r="39" spans="5:12" x14ac:dyDescent="0.25">
       <c r="F39" s="2"/>
     </row>
     <row r="40" spans="5:12" x14ac:dyDescent="0.25">
-      <c r="E40" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="F40" s="4"/>
-      <c r="G40" s="4"/>
-      <c r="H40" s="4"/>
-      <c r="I40" s="4"/>
+      <c r="E40" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="F40" s="7"/>
+      <c r="G40" s="7"/>
+      <c r="H40" s="7"/>
+      <c r="I40" s="7"/>
     </row>
     <row r="41" spans="5:12" x14ac:dyDescent="0.25">
-      <c r="F41" s="6"/>
+      <c r="F41" s="5"/>
     </row>
     <row r="42" spans="5:12" x14ac:dyDescent="0.25">
-      <c r="F42" s="8" t="s">
-        <v>12</v>
-      </c>
-      <c r="G42" s="8"/>
-      <c r="H42" s="8"/>
+      <c r="F42" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="G42" s="6"/>
+      <c r="H42" s="6"/>
     </row>
     <row r="43" spans="5:12" x14ac:dyDescent="0.25">
       <c r="F43" s="2"/>
     </row>
     <row r="44" spans="5:12" x14ac:dyDescent="0.25">
-      <c r="E44" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="F44" s="4"/>
-      <c r="G44" s="4"/>
-      <c r="H44" s="4"/>
-      <c r="I44" s="4"/>
-      <c r="J44" s="4"/>
-      <c r="K44" s="4"/>
-      <c r="L44" s="4"/>
+      <c r="E44" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="F44" s="7"/>
+      <c r="G44" s="7"/>
+      <c r="H44" s="7"/>
+      <c r="I44" s="7"/>
+      <c r="J44" s="7"/>
+      <c r="K44" s="7"/>
+      <c r="L44" s="7"/>
     </row>
     <row r="45" spans="5:12" x14ac:dyDescent="0.25">
-      <c r="F45" s="6"/>
+      <c r="F45" s="5"/>
     </row>
     <row r="46" spans="5:12" x14ac:dyDescent="0.25">
-      <c r="F46" s="8" t="s">
+      <c r="F46" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="G46" s="6"/>
+      <c r="H46" s="6"/>
+    </row>
+    <row r="47" spans="5:12" x14ac:dyDescent="0.25">
+      <c r="F47" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="G46" s="8"/>
-      <c r="H46" s="8"/>
-    </row>
-    <row r="47" spans="5:12" x14ac:dyDescent="0.25">
-      <c r="F47" s="8" t="s">
+      <c r="G47" s="6"/>
+      <c r="H47" s="6"/>
+      <c r="I47" s="6"/>
+    </row>
+    <row r="48" spans="5:12" x14ac:dyDescent="0.25">
+      <c r="F48" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="G47" s="8"/>
-      <c r="H47" s="8"/>
-      <c r="I47" s="8"/>
-    </row>
-    <row r="48" spans="5:12" x14ac:dyDescent="0.25">
-      <c r="F48" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="G48" s="8"/>
-      <c r="H48" s="8"/>
-      <c r="I48" s="8"/>
+      <c r="G48" s="6"/>
+      <c r="H48" s="6"/>
+      <c r="I48" s="6"/>
     </row>
     <row r="49" spans="5:15" x14ac:dyDescent="0.25">
       <c r="F49" s="2"/>
     </row>
     <row r="50" spans="5:15" x14ac:dyDescent="0.25">
-      <c r="E50" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="F50" s="4"/>
-      <c r="G50" s="4"/>
-      <c r="H50" s="4"/>
+      <c r="E50" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="F50" s="7"/>
+      <c r="G50" s="7"/>
+      <c r="H50" s="7"/>
     </row>
     <row r="51" spans="5:15" x14ac:dyDescent="0.25">
       <c r="F51" s="2"/>
     </row>
     <row r="52" spans="5:15" x14ac:dyDescent="0.25">
-      <c r="F52" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="G52" s="8"/>
+      <c r="F52" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="G52" s="6"/>
     </row>
     <row r="53" spans="5:15" x14ac:dyDescent="0.25">
       <c r="F53" s="2"/>
     </row>
     <row r="54" spans="5:15" x14ac:dyDescent="0.25">
-      <c r="E54" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="F54" s="4"/>
-      <c r="G54" s="4"/>
-      <c r="H54" s="4"/>
-      <c r="I54" s="4"/>
-      <c r="J54" s="4"/>
-      <c r="K54" s="4"/>
-      <c r="L54" s="4"/>
-      <c r="M54" s="4"/>
-      <c r="N54" s="4"/>
-      <c r="O54" s="4"/>
+      <c r="E54" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="F54" s="7"/>
+      <c r="G54" s="7"/>
+      <c r="H54" s="7"/>
+      <c r="I54" s="7"/>
+      <c r="J54" s="7"/>
+      <c r="K54" s="7"/>
+      <c r="L54" s="7"/>
+      <c r="M54" s="7"/>
+      <c r="N54" s="7"/>
+      <c r="O54" s="7"/>
     </row>
     <row r="56" spans="5:15" x14ac:dyDescent="0.25">
-      <c r="F56" s="8" t="s">
+      <c r="F56" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="G56" s="6"/>
+      <c r="H56" s="6"/>
+    </row>
+    <row r="57" spans="5:15" x14ac:dyDescent="0.25">
+      <c r="F57" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="G57" s="6"/>
+      <c r="H57" s="6"/>
+      <c r="I57" s="6"/>
+    </row>
+    <row r="58" spans="5:15" x14ac:dyDescent="0.25">
+      <c r="F58" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="G56" s="8"/>
-      <c r="H56" s="8"/>
-    </row>
-    <row r="57" spans="5:15" x14ac:dyDescent="0.25">
-      <c r="F57" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="G57" s="8"/>
-      <c r="H57" s="8"/>
-      <c r="I57" s="8"/>
-    </row>
-    <row r="58" spans="5:15" x14ac:dyDescent="0.25">
-      <c r="F58" s="8" t="s">
-        <v>18</v>
-      </c>
-      <c r="G58" s="8"/>
-      <c r="H58" s="8"/>
-      <c r="I58" s="8"/>
+      <c r="G58" s="6"/>
+      <c r="H58" s="6"/>
+      <c r="I58" s="6"/>
     </row>
     <row r="59" spans="5:15" x14ac:dyDescent="0.25">
       <c r="F59" s="2"/>
     </row>
     <row r="60" spans="5:15" x14ac:dyDescent="0.25">
-      <c r="E60" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="F60" s="4"/>
-      <c r="G60" s="4"/>
-      <c r="H60" s="4"/>
+      <c r="E60" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="F60" s="7"/>
+      <c r="G60" s="7"/>
+      <c r="H60" s="7"/>
     </row>
     <row r="61" spans="5:15" x14ac:dyDescent="0.25">
-      <c r="F61" s="6"/>
+      <c r="F61" s="5"/>
     </row>
     <row r="62" spans="5:15" x14ac:dyDescent="0.25">
-      <c r="F62" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="G62" s="8"/>
+      <c r="F62" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="G62" s="6"/>
     </row>
   </sheetData>
   <mergeCells count="39">
+    <mergeCell ref="B5:C5"/>
+    <mergeCell ref="B6:C6"/>
+    <mergeCell ref="B7:C7"/>
+    <mergeCell ref="B4:C4"/>
+    <mergeCell ref="B9:C9"/>
+    <mergeCell ref="F25:H25"/>
+    <mergeCell ref="F7:H7"/>
+    <mergeCell ref="F11:H11"/>
+    <mergeCell ref="F12:I12"/>
+    <mergeCell ref="E9:H9"/>
+    <mergeCell ref="E14:H14"/>
+    <mergeCell ref="E18:L18"/>
+    <mergeCell ref="E23:J23"/>
+    <mergeCell ref="F16:H16"/>
+    <mergeCell ref="F20:H20"/>
+    <mergeCell ref="F21:I21"/>
+    <mergeCell ref="F46:H46"/>
+    <mergeCell ref="F26:I26"/>
+    <mergeCell ref="E28:S28"/>
+    <mergeCell ref="F31:I31"/>
+    <mergeCell ref="F32:I32"/>
+    <mergeCell ref="F33:J33"/>
+    <mergeCell ref="E35:J35"/>
     <mergeCell ref="F57:I57"/>
     <mergeCell ref="F58:I58"/>
     <mergeCell ref="E60:H60"/>
@@ -1694,29 +1717,6 @@
     <mergeCell ref="E40:I40"/>
     <mergeCell ref="F42:H42"/>
     <mergeCell ref="E44:L44"/>
-    <mergeCell ref="F46:H46"/>
-    <mergeCell ref="F26:I26"/>
-    <mergeCell ref="E28:S28"/>
-    <mergeCell ref="F31:I31"/>
-    <mergeCell ref="F32:I32"/>
-    <mergeCell ref="F33:J33"/>
-    <mergeCell ref="E35:J35"/>
-    <mergeCell ref="E18:L18"/>
-    <mergeCell ref="E23:J23"/>
-    <mergeCell ref="F16:H16"/>
-    <mergeCell ref="F20:H20"/>
-    <mergeCell ref="F21:I21"/>
-    <mergeCell ref="F25:H25"/>
-    <mergeCell ref="F7:H7"/>
-    <mergeCell ref="F11:H11"/>
-    <mergeCell ref="F12:I12"/>
-    <mergeCell ref="E9:H9"/>
-    <mergeCell ref="E14:H14"/>
-    <mergeCell ref="B5:C5"/>
-    <mergeCell ref="B6:C6"/>
-    <mergeCell ref="B7:C7"/>
-    <mergeCell ref="B4:C4"/>
-    <mergeCell ref="B9:C9"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>